<commit_message>
Added template for interviews and first data
</commit_message>
<xml_diff>
--- a/MicroDepGraph/Data analysis.xlsx
+++ b/MicroDepGraph/Data analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Escritorio\Universidad\SWME\SME-Group1\MicroDepGraph\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52F81EC4-7F7E-4AAB-9A76-3DFB285DD4FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4F1D313-C3F8-4F54-9731-3284A007CB59}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6240" yWindow="9420" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
   <si>
     <t>PROJECTS NAME</t>
   </si>
@@ -75,6 +75,48 @@
   </si>
   <si>
     <t>data-services-javaee7</t>
+  </si>
+  <si>
+    <t>e-ground-2019</t>
+  </si>
+  <si>
+    <t>empathy_delivery</t>
+  </si>
+  <si>
+    <t>LakesideMutual</t>
+  </si>
+  <si>
+    <t>lelylan</t>
+  </si>
+  <si>
+    <t>Microservices-Demo</t>
+  </si>
+  <si>
+    <t>odm-ondocker</t>
+  </si>
+  <si>
+    <t>rsa</t>
+  </si>
+  <si>
+    <t>springboot-graphql-databases</t>
+  </si>
+  <si>
+    <t>spring-petclinic-microservices</t>
+  </si>
+  <si>
+    <t>event-sourcing-microservices-example</t>
+  </si>
+  <si>
+    <t>LearnMicro</t>
+  </si>
+  <si>
+    <t>spring-cloud-microservice-examples</t>
+  </si>
+  <si>
+    <t>spring-cloud-netflix-example</t>
+  </si>
+  <si>
+    <t>eShopOnContainers-dev</t>
   </si>
 </sst>
 </file>
@@ -425,12 +467,12 @@
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="B18" sqref="A1:B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.28515625" customWidth="1"/>
+    <col min="1" max="1" width="35.42578125" customWidth="1"/>
     <col min="2" max="2" width="25.85546875" customWidth="1"/>
     <col min="3" max="3" width="28.140625" customWidth="1"/>
     <col min="4" max="4" width="34.28515625" customWidth="1"/>
@@ -485,21 +527,21 @@
         <v>7</v>
       </c>
       <c r="D2" s="1">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E2" s="1">
         <f>C2/D2</f>
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="F2" s="1">
         <v>11</v>
       </c>
       <c r="G2" s="1">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="H2" s="1">
         <f>F2/G2</f>
-        <v>2.75</v>
+        <v>1.375</v>
       </c>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
@@ -553,7 +595,9 @@
       <c r="J4" s="1"/>
     </row>
     <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="3"/>
+      <c r="A5" s="3" t="s">
+        <v>14</v>
+      </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -571,7 +615,9 @@
       <c r="J5" s="3"/>
     </row>
     <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="1"/>
+      <c r="A6" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -589,7 +635,9 @@
       <c r="J6" s="1"/>
     </row>
     <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="3"/>
+      <c r="A7" s="3" t="s">
+        <v>16</v>
+      </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
@@ -607,7 +655,9 @@
       <c r="J7" s="3"/>
     </row>
     <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="1"/>
+      <c r="A8" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -625,7 +675,9 @@
       <c r="J8" s="1"/>
     </row>
     <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="3"/>
+      <c r="A9" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
@@ -643,7 +695,9 @@
       <c r="J9" s="3"/>
     </row>
     <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="1"/>
+      <c r="A10" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -661,7 +715,9 @@
       <c r="J10" s="1"/>
     </row>
     <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="3"/>
+      <c r="A11" s="3" t="s">
+        <v>20</v>
+      </c>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
@@ -679,7 +735,9 @@
       <c r="J11" s="3"/>
     </row>
     <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="1"/>
+      <c r="A12" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -697,7 +755,9 @@
       <c r="J12" s="1"/>
     </row>
     <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="3"/>
+      <c r="A13" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
@@ -715,7 +775,9 @@
       <c r="J13" s="3"/>
     </row>
     <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="1"/>
+      <c r="A14" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -733,7 +795,9 @@
       <c r="J14" s="1"/>
     </row>
     <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="3"/>
+      <c r="A15" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
@@ -751,7 +815,9 @@
       <c r="J15" s="3"/>
     </row>
     <row r="16" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="1"/>
+      <c r="A16" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -769,7 +835,9 @@
       <c r="J16" s="1"/>
     </row>
     <row r="17" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="3"/>
+      <c r="A17" s="3" t="s">
+        <v>26</v>
+      </c>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
@@ -787,7 +855,9 @@
       <c r="J17" s="3"/>
     </row>
     <row r="18" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="1"/>
+      <c r="A18" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>

</xml_diff>